<commit_message>
updated dec 2025 cpi and arrivals
</commit_message>
<xml_diff>
--- a/inflation_2012-24.xlsx
+++ b/inflation_2012-24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RBI Official\DCA\Dashboard\Inflation-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8CDD10-5BAE-401C-979D-CD6F60B284E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F828F194-8C32-4108-BAC0-7FE2A354D778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3EA9A55A-B48B-4035-99BE-2980B3C8C172}"/>
   </bookViews>
@@ -658,13 +658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DBFB1-5D6A-4B75-89EE-EC9E4D2C9668}">
-  <dimension ref="A1:FC29"/>
+  <dimension ref="A1:FD29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="EH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="EO2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FB29" sqref="FB29:FC29"/>
+      <selection pane="bottomRight" activeCell="FF20" sqref="FF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,7 +672,7 @@
     <col min="1" max="1" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:160" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1150,8 +1150,11 @@
       <c r="FC1" s="16">
         <v>45597</v>
       </c>
+      <c r="FD1" s="16">
+        <v>45627</v>
+      </c>
     </row>
-    <row r="2" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1629,8 +1632,11 @@
       <c r="FC2" s="4">
         <v>6.8797399783315365</v>
       </c>
+      <c r="FD2" s="4">
+        <v>6.5053763440860184</v>
+      </c>
     </row>
-    <row r="3" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2108,8 +2114,11 @@
       <c r="FC3" s="4">
         <v>4.6728971962616823</v>
       </c>
+      <c r="FD3" s="4">
+        <v>5.3005205868433451</v>
+      </c>
     </row>
-    <row r="4" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2587,8 +2596,11 @@
       <c r="FC4" s="4">
         <v>4.8412285268089601</v>
       </c>
+      <c r="FD4" s="4">
+        <v>6.8513853904282094</v>
+      </c>
     </row>
-    <row r="5" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3066,8 +3078,11 @@
       <c r="FC5" s="4">
         <v>2.8540065861690547</v>
       </c>
+      <c r="FD5" s="4">
+        <v>2.7960526315789442</v>
+      </c>
     </row>
-    <row r="6" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -3545,8 +3560,11 @@
       <c r="FC6" s="8">
         <v>13.2793017456359</v>
       </c>
+      <c r="FD6" s="8">
+        <v>14.597629444791002</v>
+      </c>
     </row>
-    <row r="7" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -4024,8 +4042,11 @@
       <c r="FC7" s="4">
         <v>7.6793721973094105</v>
       </c>
+      <c r="FD7" s="4">
+        <v>8.490028490028493</v>
+      </c>
     </row>
-    <row r="8" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -4501,10 +4522,13 @@
         <v>42.230881636629313</v>
       </c>
       <c r="FC8" s="4">
-        <v>29.32714617169373</v>
+        <v>29.373549883990723</v>
+      </c>
+      <c r="FD8" s="4">
+        <v>26.555609995100447</v>
       </c>
     </row>
-    <row r="9" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -4982,8 +5006,11 @@
       <c r="FC9" s="8">
         <v>5.4119941491955119</v>
       </c>
+      <c r="FD9" s="8">
+        <v>3.8312318137730386</v>
+      </c>
     </row>
-    <row r="10" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -5461,8 +5488,11 @@
       <c r="FC10" s="4">
         <v>1.3066871637202282</v>
       </c>
+      <c r="FD10" s="4">
+        <v>0.30627871362940712</v>
+      </c>
     </row>
-    <row r="11" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -5940,8 +5970,11 @@
       <c r="FC11" s="4">
         <v>-7.4269480519480569</v>
       </c>
+      <c r="FD11" s="4">
+        <v>-7.4104234527687245</v>
+      </c>
     </row>
-    <row r="12" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -6419,8 +6452,11 @@
       <c r="FC12" s="4">
         <v>2.7195467422096384</v>
       </c>
+      <c r="FD12" s="4">
+        <v>3.0560271646859118</v>
+      </c>
     </row>
-    <row r="13" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -6898,8 +6934,11 @@
       <c r="FC13" s="4">
         <v>3.9493670886076004</v>
       </c>
+      <c r="FD13" s="4">
+        <v>3.987884906612825</v>
+      </c>
     </row>
-    <row r="14" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -7377,8 +7416,11 @@
       <c r="FC14" s="9">
         <v>8.2035306334371807</v>
       </c>
+      <c r="FD14" s="9">
+        <v>7.6882845188284614</v>
+      </c>
     </row>
-    <row r="15" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
@@ -7856,8 +7898,11 @@
       <c r="FC15" s="8">
         <v>2.3483365949119288</v>
       </c>
+      <c r="FD15" s="8">
+        <v>2.4938875305623442</v>
+      </c>
     </row>
-    <row r="16" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -8333,10 +8378,13 @@
         <v>2.7894736842105323</v>
       </c>
       <c r="FC16" s="4">
-        <v>2.8346456692913415</v>
+        <v>2.7821522309711346</v>
+      </c>
+      <c r="FD16" s="4">
+        <v>2.7763226820324687</v>
       </c>
     </row>
-    <row r="17" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -8812,10 +8860,13 @@
         <v>2.1475770925110163</v>
       </c>
       <c r="FC17" s="4">
-        <v>2.1428571428571459</v>
+        <v>2.197802197802198</v>
+      </c>
+      <c r="FD17" s="4">
+        <v>2.0285087719298183</v>
       </c>
     </row>
-    <row r="18" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -9293,8 +9344,11 @@
       <c r="FC18" s="8">
         <v>2.7484143763213624</v>
       </c>
+      <c r="FD18" s="8">
+        <v>2.7426160337552834</v>
+      </c>
     </row>
-    <row r="19" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -9772,8 +9826,11 @@
       <c r="FC19" s="8">
         <v>2.8667790893760503</v>
       </c>
+      <c r="FD19" s="8">
+        <v>2.7133973996608156</v>
+      </c>
     </row>
-    <row r="20" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
@@ -10251,8 +10308,11 @@
       <c r="FC20" s="9">
         <v>-1.8343524180100119</v>
       </c>
+      <c r="FD20" s="9">
+        <v>-1.3873473917869035</v>
+      </c>
     </row>
-    <row r="21" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -10730,8 +10790,11 @@
       <c r="FC21" s="4">
         <v>2.818489289740699</v>
       </c>
+      <c r="FD21" s="4">
+        <v>2.7543563799887609</v>
+      </c>
     </row>
-    <row r="22" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -11209,8 +11272,11 @@
       <c r="FC22" s="4">
         <v>4.0063257775435019</v>
       </c>
+      <c r="FD22" s="4">
+        <v>4.0462427745664682</v>
+      </c>
     </row>
-    <row r="23" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -11686,10 +11752,13 @@
         <v>2.7694160144491238</v>
       </c>
       <c r="FC23" s="4">
-        <v>2.6442307692307727</v>
+        <v>2.7043269230769229</v>
+      </c>
+      <c r="FD23" s="4">
+        <v>2.6410564225690312</v>
       </c>
     </row>
-    <row r="24" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -12167,8 +12236,11 @@
       <c r="FC24" s="4">
         <v>2.6467203682393521</v>
       </c>
+      <c r="FD24" s="4">
+        <v>2.6995979322228703</v>
+      </c>
     </row>
-    <row r="25" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -12646,8 +12718,11 @@
       <c r="FC25" s="4">
         <v>3.8925438596491198</v>
       </c>
+      <c r="FD25" s="4">
+        <v>3.8904109589041065</v>
+      </c>
     </row>
-    <row r="26" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -13125,8 +13200,11 @@
       <c r="FC26" s="4">
         <v>10.416666666666668</v>
       </c>
+      <c r="FD26" s="4">
+        <v>9.7030752916224863</v>
+      </c>
     </row>
-    <row r="27" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -13604,8 +13682,11 @@
       <c r="FC27" s="8">
         <v>4.2553191489361675</v>
       </c>
+      <c r="FD27" s="8">
+        <v>4.1899441340782122</v>
+      </c>
     </row>
-    <row r="28" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
@@ -14083,8 +14164,11 @@
       <c r="FC28" s="9">
         <v>5.4750402576489474</v>
       </c>
+      <c r="FD28" s="9">
+        <v>5.2234787291330198</v>
+      </c>
     </row>
-    <row r="29" spans="1:159" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:160" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>48</v>
       </c>
@@ -14561,6 +14645,9 @@
       </c>
       <c r="FC29" s="15">
         <v>3.7117969176061103</v>
+      </c>
+      <c r="FD29" s="15">
+        <v>3.6522114599136022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated march inflation data
</commit_message>
<xml_diff>
--- a/inflation_2012-24.xlsx
+++ b/inflation_2012-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RBI Official\DCA\Dashboard\Inflation-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFDF9B3-B5F8-4058-ACA3-8E95D388FACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE27135-E381-44F3-9B6E-C494A0B79D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3EA9A55A-B48B-4035-99BE-2980B3C8C172}"/>
   </bookViews>
@@ -658,13 +658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DBFB1-5D6A-4B75-89EE-EC9E4D2C9668}">
-  <dimension ref="A1:FE29"/>
+  <dimension ref="A1:FG29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="EN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="EM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FI21" sqref="FI21"/>
+      <selection pane="bottomRight" activeCell="FJ24" sqref="FJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,7 +672,7 @@
     <col min="1" max="1" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:161" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1156,8 +1156,14 @@
       <c r="FE1" s="16">
         <v>45658</v>
       </c>
+      <c r="FF1" s="16">
+        <v>45689</v>
+      </c>
+      <c r="FG1" s="16">
+        <v>45717</v>
+      </c>
     </row>
-    <row r="2" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1641,8 +1647,14 @@
       <c r="FE2" s="4">
         <v>6.243329775880464</v>
       </c>
+      <c r="FF2" s="4">
+        <v>6.1007957559681696</v>
+      </c>
+      <c r="FG2" s="4">
+        <v>5.9259259259259203</v>
+      </c>
     </row>
-    <row r="3" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2126,8 +2138,14 @@
       <c r="FE3" s="4">
         <v>5.2532833020637977</v>
       </c>
+      <c r="FF3" s="4">
+        <v>2.1100917431192636</v>
+      </c>
+      <c r="FG3" s="4">
+        <v>0.31674208144795862</v>
+      </c>
     </row>
-    <row r="4" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2611,8 +2629,14 @@
       <c r="FE4" s="4">
         <v>1.2664393570384773</v>
       </c>
+      <c r="FF4" s="4">
+        <v>-2.9571217348447512</v>
+      </c>
+      <c r="FG4" s="4">
+        <v>-3.1557165028453302</v>
+      </c>
     </row>
-    <row r="5" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3096,8 +3120,14 @@
       <c r="FE5" s="4">
         <v>2.8461959496442351</v>
       </c>
+      <c r="FF5" s="4">
+        <v>2.677595628415304</v>
+      </c>
+      <c r="FG5" s="4">
+        <v>2.5641025641025577</v>
+      </c>
     </row>
-    <row r="6" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -3581,8 +3611,14 @@
       <c r="FE6" s="8">
         <v>15.640703517587944</v>
       </c>
+      <c r="FF6" s="8">
+        <v>16.361339229311419</v>
+      </c>
+      <c r="FG6" s="8">
+        <v>17.06700379266751</v>
+      </c>
     </row>
-    <row r="7" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -4064,10 +4100,16 @@
         <v>8.6039886039886007</v>
       </c>
       <c r="FE7" s="4">
-        <v>12.216404886561955</v>
+        <v>12.158231529959282</v>
+      </c>
+      <c r="FF7" s="4">
+        <v>14.819136522753794</v>
+      </c>
+      <c r="FG7" s="4">
+        <v>16.265750286368846</v>
       </c>
     </row>
-    <row r="8" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -4551,8 +4593,14 @@
       <c r="FE8" s="4">
         <v>11.349693251533752</v>
       </c>
+      <c r="FF8" s="4">
+        <v>-1.1253196930946234</v>
+      </c>
+      <c r="FG8" s="4">
+        <v>-7.0372259051504251</v>
+      </c>
     </row>
-    <row r="9" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -5034,10 +5082,16 @@
         <v>3.8312318137730386</v>
       </c>
       <c r="FE9" s="8">
-        <v>2.5942241801272554</v>
+        <v>2.5452765540871209</v>
+      </c>
+      <c r="FF9" s="8">
+        <v>-0.34550839091805957</v>
+      </c>
+      <c r="FG9" s="8">
+        <v>-2.7295285359801489</v>
       </c>
     </row>
-    <row r="10" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -5521,8 +5575,14 @@
       <c r="FE10" s="4">
         <v>0.3074558032282903</v>
       </c>
+      <c r="FF10" s="4">
+        <v>2.1638330757341442</v>
+      </c>
+      <c r="FG10" s="4">
+        <v>3.8850038850038855</v>
+      </c>
     </row>
-    <row r="11" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -6006,8 +6066,14 @@
       <c r="FE11" s="4">
         <v>-6.8481848184818448</v>
       </c>
+      <c r="FF11" s="4">
+        <v>-5.8452481076534921</v>
+      </c>
+      <c r="FG11" s="4">
+        <v>-4.9229452054794525</v>
+      </c>
     </row>
-    <row r="12" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -6491,8 +6557,14 @@
       <c r="FE12" s="4">
         <v>3.3879164313946921</v>
       </c>
+      <c r="FF12" s="4">
+        <v>3.7267080745341583</v>
+      </c>
+      <c r="FG12" s="4">
+        <v>4.0067720090293584</v>
+      </c>
     </row>
-    <row r="13" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -6976,8 +7048,14 @@
       <c r="FE13" s="4">
         <v>4.0744466800804799</v>
       </c>
+      <c r="FF13" s="4">
+        <v>4.2126379137412258</v>
+      </c>
+      <c r="FG13" s="4">
+        <v>4.3021510755377665</v>
+      </c>
     </row>
-    <row r="14" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -7461,8 +7539,14 @@
       <c r="FE14" s="9">
         <v>5.6812204103103694</v>
       </c>
+      <c r="FF14" s="9">
+        <v>3.8360483447188556</v>
+      </c>
+      <c r="FG14" s="9">
+        <v>2.8841111693759833</v>
+      </c>
     </row>
-    <row r="15" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
@@ -7946,8 +8030,14 @@
       <c r="FE15" s="8">
         <v>2.296042989741093</v>
       </c>
+      <c r="FF15" s="8">
+        <v>2.4366471734892792</v>
+      </c>
+      <c r="FG15" s="8">
+        <v>2.4793388429752179</v>
+      </c>
     </row>
-    <row r="16" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -8431,8 +8521,14 @@
       <c r="FE16" s="4">
         <v>2.7182435964453679</v>
       </c>
+      <c r="FF16" s="4">
+        <v>2.7676240208877343</v>
+      </c>
+      <c r="FG16" s="4">
+        <v>2.7097446586763878</v>
+      </c>
     </row>
-    <row r="17" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -8916,8 +9012,14 @@
       <c r="FE17" s="4">
         <v>2.0799124247400171</v>
       </c>
+      <c r="FF17" s="4">
+        <v>2.0218579234972616</v>
+      </c>
+      <c r="FG17" s="4">
+        <v>2.0185488270594591</v>
+      </c>
     </row>
-    <row r="18" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -9401,8 +9503,14 @@
       <c r="FE18" s="8">
         <v>2.6842105263157867</v>
       </c>
+      <c r="FF18" s="8">
+        <v>2.6799789805570122</v>
+      </c>
+      <c r="FG18" s="8">
+        <v>2.6232948583420774</v>
+      </c>
     </row>
-    <row r="19" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -9884,10 +9992,16 @@
         <v>2.7133973996608156</v>
       </c>
       <c r="FE19" s="8">
-        <v>2.7590090090090125</v>
+        <v>2.8153153153153152</v>
+      </c>
+      <c r="FF19" s="8">
+        <v>2.9131652661064362</v>
+      </c>
+      <c r="FG19" s="8">
+        <v>3.0303030303030338</v>
       </c>
     </row>
-    <row r="20" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
@@ -10369,10 +10483,16 @@
         <v>-1.3318534961154147</v>
       </c>
       <c r="FE20" s="9">
-        <v>-1.3819789939192924</v>
+        <v>-1.4925373134328452</v>
+      </c>
+      <c r="FF20" s="9">
+        <v>-1.3281682346430421</v>
+      </c>
+      <c r="FG20" s="9">
+        <v>1.4789533560864587</v>
       </c>
     </row>
-    <row r="21" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -10856,8 +10976,14 @@
       <c r="FE21" s="4">
         <v>2.8619528619528749</v>
       </c>
+      <c r="FF21" s="4">
+        <v>2.7995520716685331</v>
+      </c>
+      <c r="FG21" s="4">
+        <v>2.6830631637786375</v>
+      </c>
     </row>
-    <row r="22" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -11341,8 +11467,14 @@
       <c r="FE22" s="4">
         <v>3.974895397489552</v>
       </c>
+      <c r="FF22" s="4">
+        <v>4.121022430881589</v>
+      </c>
+      <c r="FG22" s="4">
+        <v>4.264170566822667</v>
+      </c>
     </row>
-    <row r="23" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -11826,8 +11958,14 @@
       <c r="FE23" s="4">
         <v>2.7577937649880058</v>
       </c>
+      <c r="FF23" s="4">
+        <v>2.9341317365269495</v>
+      </c>
+      <c r="FG23" s="4">
+        <v>3.2993401319736058</v>
+      </c>
     </row>
-    <row r="24" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -12309,10 +12447,16 @@
         <v>2.6995979322228703</v>
       </c>
       <c r="FE24" s="4">
-        <v>2.6376146788990793</v>
+        <v>2.6949541284403606</v>
+      </c>
+      <c r="FF24" s="4">
+        <v>2.6918671248568256</v>
+      </c>
+      <c r="FG24" s="4">
+        <v>2.3999999999999932</v>
       </c>
     </row>
-    <row r="25" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -12796,8 +12940,14 @@
       <c r="FE25" s="4">
         <v>3.8272279934390379</v>
       </c>
+      <c r="FF25" s="4">
+        <v>3.8251366120218582</v>
+      </c>
+      <c r="FG25" s="4">
+        <v>3.9847161572052467</v>
+      </c>
     </row>
-    <row r="26" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -13279,10 +13429,16 @@
         <v>9.7560975609756131</v>
       </c>
       <c r="FE26" s="4">
-        <v>10.576414595452142</v>
+        <v>10.629296668429401</v>
+      </c>
+      <c r="FF26" s="4">
+        <v>13.629160063391431</v>
+      </c>
+      <c r="FG26" s="4">
+        <v>13.496612819176656</v>
       </c>
     </row>
-    <row r="27" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -13766,8 +13922,14 @@
       <c r="FE27" s="8">
         <v>4.3478260869565117</v>
       </c>
+      <c r="FF27" s="8">
+        <v>4.8387096774193488</v>
+      </c>
+      <c r="FG27" s="8">
+        <v>4.9944506104328523</v>
+      </c>
     </row>
-    <row r="28" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
@@ -14249,10 +14411,16 @@
         <v>5.2234787291330198</v>
       </c>
       <c r="FE28" s="9">
-        <v>4.3126684636118604</v>
+        <v>4.2587601078167152</v>
+      </c>
+      <c r="FF28" s="9">
+        <v>3.6060279870828786</v>
+      </c>
+      <c r="FG28" s="9">
+        <v>3.3369214208826632</v>
       </c>
     </row>
-    <row r="29" spans="1:161" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:163" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>48</v>
       </c>
@@ -14734,7 +14902,13 @@
         <v>3.6442291982728143</v>
       </c>
       <c r="FE29" s="15">
-        <v>3.7443258358855038</v>
+        <v>3.6438913567008466</v>
+      </c>
+      <c r="FF29" s="15">
+        <v>4.0808165021712144</v>
+      </c>
+      <c r="FG29" s="15">
+        <v>4.0545058599220907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated cpi, arrivals and agri data
</commit_message>
<xml_diff>
--- a/inflation_2012-24.xlsx
+++ b/inflation_2012-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RBI Official\DCA\Dashboard\Inflation-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496C877A-B260-4BEA-AA8F-F38E622ECE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D07FE5-D88E-435B-87E8-DEA798876D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="70" windowWidth="19180" windowHeight="11260" xr2:uid="{3EA9A55A-B48B-4035-99BE-2980B3C8C172}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3EA9A55A-B48B-4035-99BE-2980B3C8C172}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -658,13 +658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DBFB1-5D6A-4B75-89EE-EC9E4D2C9668}">
-  <dimension ref="A1:FH29"/>
+  <dimension ref="A1:FI29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="EL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="ES2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FH2" sqref="FH2:FH29"/>
+      <selection pane="bottomRight" activeCell="FM12" sqref="FM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,7 +672,7 @@
     <col min="1" max="1" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:164" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:165" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1165,8 +1165,11 @@
       <c r="FH1" s="16">
         <v>45748</v>
       </c>
+      <c r="FI1" s="16">
+        <v>45778</v>
+      </c>
     </row>
-    <row r="2" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1659,8 +1662,11 @@
       <c r="FH2" s="4">
         <v>5.3495762711864376</v>
       </c>
+      <c r="FI2" s="4">
+        <v>4.7669491525423728</v>
+      </c>
     </row>
-    <row r="3" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2153,8 +2159,11 @@
       <c r="FH3" s="4">
         <v>-0.35320088300221253</v>
       </c>
+      <c r="FI3" s="4">
+        <v>-0.39147455415398241</v>
+      </c>
     </row>
-    <row r="4" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2647,8 +2656,11 @@
       <c r="FH4" s="4">
         <v>0.82553659878921293</v>
       </c>
+      <c r="FI4" s="4">
+        <v>0.64343163538873382</v>
+      </c>
     </row>
-    <row r="5" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3141,8 +3153,11 @@
       <c r="FH5" s="4">
         <v>2.7218290691344587</v>
       </c>
+      <c r="FI5" s="4">
+        <v>3.1487513572204189</v>
+      </c>
     </row>
-    <row r="6" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -3635,8 +3650,11 @@
       <c r="FH6" s="8">
         <v>17.424242424242419</v>
       </c>
+      <c r="FI6" s="8">
+        <v>17.906683480453978</v>
+      </c>
     </row>
-    <row r="7" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -4127,10 +4145,13 @@
         <v>16.265750286368846</v>
       </c>
       <c r="FH7" s="4">
-        <v>13.800539083557947</v>
+        <v>13.908355795148253</v>
+      </c>
+      <c r="FI7" s="4">
+        <v>12.738160043549268</v>
       </c>
     </row>
-    <row r="8" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -4623,8 +4644,11 @@
       <c r="FH8" s="4">
         <v>-10.97683786505538</v>
       </c>
+      <c r="FI8" s="4">
+        <v>-13.700633837152607</v>
+      </c>
     </row>
-    <row r="9" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -5117,8 +5141,11 @@
       <c r="FH9" s="8">
         <v>-5.231984205330698</v>
       </c>
+      <c r="FI9" s="8">
+        <v>-8.2158483228001842</v>
+      </c>
     </row>
-    <row r="10" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -5611,8 +5638,11 @@
       <c r="FH10" s="4">
         <v>4.5878693623639233</v>
       </c>
+      <c r="FI10" s="4">
+        <v>4.0863531225906025</v>
+      </c>
     </row>
-    <row r="11" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -6103,10 +6133,13 @@
         <v>-4.9229452054794525</v>
       </c>
       <c r="FH11" s="4">
-        <v>-3.4001743679163079</v>
+        <v>-3.443766346992156</v>
+      </c>
+      <c r="FI11" s="4">
+        <v>-2.8156621205455368</v>
       </c>
     </row>
-    <row r="12" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -6599,8 +6632,11 @@
       <c r="FH12" s="4">
         <v>4.3968432919954807</v>
       </c>
+      <c r="FI12" s="4">
+        <v>4.5608108108108079</v>
+      </c>
     </row>
-    <row r="13" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -7091,10 +7127,13 @@
         <v>4.3021510755377665</v>
       </c>
       <c r="FH13" s="4">
-        <v>4.3956043956044013</v>
+        <v>4.445554445554448</v>
+      </c>
+      <c r="FI13" s="4">
+        <v>4.384653712007978</v>
       </c>
     </row>
-    <row r="14" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -7587,8 +7626,11 @@
       <c r="FH14" s="9">
         <v>2.1365294424179231</v>
       </c>
+      <c r="FI14" s="9">
+        <v>1.5010351966873736</v>
+      </c>
     </row>
-    <row r="15" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
@@ -8081,8 +8123,11 @@
       <c r="FH15" s="8">
         <v>2.0813165537270142</v>
       </c>
+      <c r="FI15" s="8">
+        <v>2.4142926122646067</v>
+      </c>
     </row>
-    <row r="16" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -8575,8 +8620,11 @@
       <c r="FH16" s="4">
         <v>2.7041081643265672</v>
       </c>
+      <c r="FI16" s="4">
+        <v>2.8037383177570123</v>
+      </c>
     </row>
-    <row r="17" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -9069,8 +9117,11 @@
       <c r="FH17" s="4">
         <v>2.0708446866485075</v>
       </c>
+      <c r="FI17" s="4">
+        <v>2.1786492374727668</v>
+      </c>
     </row>
-    <row r="18" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -9563,8 +9614,11 @@
       <c r="FH18" s="8">
         <v>2.6701570680628244</v>
       </c>
+      <c r="FI18" s="8">
+        <v>2.6659696811291136</v>
+      </c>
     </row>
-    <row r="19" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -10055,10 +10109,13 @@
         <v>3.0303030303030338</v>
       </c>
       <c r="FH19" s="8">
-        <v>3.0016675931072849</v>
+        <v>3.0572540300166757</v>
+      </c>
+      <c r="FI19" s="8">
+        <v>3.1649083842309924</v>
       </c>
     </row>
-    <row r="20" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
@@ -10551,8 +10608,11 @@
       <c r="FH20" s="9">
         <v>2.9243119266055011</v>
       </c>
+      <c r="FI20" s="9">
+        <v>2.7825099375354942</v>
+      </c>
     </row>
-    <row r="21" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -11045,8 +11105,11 @@
       <c r="FH21" s="4">
         <v>2.508361204013378</v>
       </c>
+      <c r="FI21" s="4">
+        <v>2.0044543429844066</v>
+      </c>
     </row>
-    <row r="22" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -11539,8 +11602,11 @@
       <c r="FH22" s="4">
         <v>4.2509072058061115</v>
       </c>
+      <c r="FI22" s="4">
+        <v>4.3410852713178318</v>
+      </c>
     </row>
-    <row r="23" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -12031,10 +12097,13 @@
         <v>3.3593281343731394</v>
       </c>
       <c r="FH23" s="4">
-        <v>3.7282020444978885</v>
+        <v>3.6680697534576026</v>
+      </c>
+      <c r="FI23" s="4">
+        <v>3.8461538461538494</v>
       </c>
     </row>
-    <row r="24" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -12527,8 +12596,11 @@
       <c r="FH24" s="4">
         <v>2.5114155251141588</v>
       </c>
+      <c r="FI24" s="4">
+        <v>2.4487471526195965</v>
+      </c>
     </row>
-    <row r="25" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -13021,8 +13093,11 @@
       <c r="FH25" s="4">
         <v>4.1349292709466781</v>
       </c>
+      <c r="FI25" s="4">
+        <v>4.1237113402061816</v>
+      </c>
     </row>
-    <row r="26" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -13513,10 +13588,13 @@
         <v>13.496612819176656</v>
       </c>
       <c r="FH26" s="4">
-        <v>12.898330804248861</v>
+        <v>12.9489124936773</v>
+      </c>
+      <c r="FI26" s="4">
+        <v>13.49047141424273</v>
       </c>
     </row>
-    <row r="27" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -14009,8 +14087,11 @@
       <c r="FH27" s="8">
         <v>5.022075055187651</v>
       </c>
+      <c r="FI27" s="8">
+        <v>5.0632911392405155</v>
+      </c>
     </row>
-    <row r="28" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
@@ -14503,8 +14584,11 @@
       <c r="FH28" s="9">
         <v>3.1601499732190717</v>
       </c>
+      <c r="FI28" s="9">
+        <v>2.8236547682472093</v>
+      </c>
     </row>
-    <row r="29" spans="1:164" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:165" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>48</v>
       </c>
@@ -14996,6 +15080,9 @@
       </c>
       <c r="FH29" s="15">
         <v>4.2308193214599834</v>
+      </c>
+      <c r="FI29" s="15">
+        <v>4.1754907686376965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated arrivals and july cpi
</commit_message>
<xml_diff>
--- a/inflation_2012-24.xlsx
+++ b/inflation_2012-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RBI Official\DCA\Dashboard\Inflation-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8CCD09-5C40-43CE-873C-3427AC17B372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC922CD-DD10-4678-B269-842C7DA1D801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3EA9A55A-B48B-4035-99BE-2980B3C8C172}"/>
   </bookViews>
@@ -658,13 +658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DBFB1-5D6A-4B75-89EE-EC9E4D2C9668}">
-  <dimension ref="A1:FJ29"/>
+  <dimension ref="A1:FK29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="ER2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="EQ2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FJ2" sqref="FJ2:FJ29"/>
+      <selection pane="bottomRight" activeCell="FN7" sqref="FN7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,7 +672,7 @@
     <col min="1" max="1" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:166" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:167" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1171,8 +1171,11 @@
       <c r="FJ1" s="16">
         <v>45809</v>
       </c>
+      <c r="FK1" s="16">
+        <v>45839</v>
+      </c>
     </row>
-    <row r="2" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1671,8 +1674,11 @@
       <c r="FJ2" s="4">
         <v>3.7348763808521803</v>
       </c>
+      <c r="FK2" s="4">
+        <v>3.0318870883429079</v>
+      </c>
     </row>
-    <row r="3" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2171,8 +2177,11 @@
       <c r="FJ3" s="4">
         <v>-1.6197783461210498</v>
       </c>
+      <c r="FK3" s="4">
+        <v>-0.60684872128304179</v>
+      </c>
     </row>
-    <row r="4" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2671,8 +2680,11 @@
       <c r="FJ4" s="4">
         <v>2.5748817656331986</v>
       </c>
+      <c r="FK4" s="4">
+        <v>2.2645393721049802</v>
+      </c>
     </row>
-    <row r="5" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3171,8 +3183,11 @@
       <c r="FJ5" s="4">
         <v>2.8047464940668765</v>
       </c>
+      <c r="FK5" s="4">
+        <v>2.7419354838709649</v>
+      </c>
     </row>
-    <row r="6" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -3671,8 +3686,11 @@
       <c r="FJ6" s="8">
         <v>17.750000000000004</v>
       </c>
+      <c r="FK6" s="8">
+        <v>19.242706393544385</v>
+      </c>
     </row>
-    <row r="7" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -4169,10 +4187,13 @@
         <v>12.738160043549268</v>
       </c>
       <c r="FJ7" s="4">
-        <v>12.588171459576769</v>
+        <v>12.642430819316322</v>
+      </c>
+      <c r="FK7" s="4">
+        <v>14.423592493297591</v>
       </c>
     </row>
-    <row r="8" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -4669,10 +4690,13 @@
         <v>-13.700633837152607</v>
       </c>
       <c r="FJ8" s="4">
-        <v>-19.000853970964986</v>
+        <v>-18.915456874466262</v>
+      </c>
+      <c r="FK8" s="4">
+        <v>-20.688365132809579</v>
       </c>
     </row>
-    <row r="9" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -5171,8 +5195,11 @@
       <c r="FJ9" s="8">
         <v>-11.759127548601239</v>
       </c>
+      <c r="FK9" s="8">
+        <v>-13.757604117922313</v>
+      </c>
     </row>
-    <row r="10" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -5671,8 +5698,11 @@
       <c r="FJ10" s="4">
         <v>3.5195103289977223</v>
       </c>
+      <c r="FK10" s="4">
+        <v>3.2824427480916114</v>
+      </c>
     </row>
-    <row r="11" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -6171,8 +6201,11 @@
       <c r="FJ11" s="4">
         <v>-3.0303030303030205</v>
       </c>
+      <c r="FK11" s="4">
+        <v>-3.0715225976305396</v>
+      </c>
     </row>
-    <row r="12" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -6671,8 +6704,11 @@
       <c r="FJ12" s="4">
         <v>4.3234138124649171</v>
       </c>
+      <c r="FK12" s="4">
+        <v>4.5964125560538047</v>
+      </c>
     </row>
-    <row r="13" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -7171,8 +7207,11 @@
       <c r="FJ13" s="4">
         <v>4.3176178660049569</v>
       </c>
+      <c r="FK13" s="4">
+        <v>4.3542800593765518</v>
+      </c>
     </row>
-    <row r="14" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -7669,10 +7708,13 @@
         <v>1.5010351966873736</v>
       </c>
       <c r="FJ14" s="9">
-        <v>-0.2016129032258093</v>
+        <v>-0.15120967741936056</v>
+      </c>
+      <c r="FK14" s="9">
+        <v>-0.83620265617315148</v>
       </c>
     </row>
-    <row r="15" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
@@ -8171,8 +8213,11 @@
       <c r="FJ15" s="8">
         <v>2.407318247472316</v>
       </c>
+      <c r="FK15" s="8">
+        <v>2.4495677233429505</v>
+      </c>
     </row>
-    <row r="16" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -8671,8 +8716,11 @@
       <c r="FJ16" s="4">
         <v>2.639751552795043</v>
       </c>
+      <c r="FK16" s="4">
+        <v>2.5826446280991737</v>
+      </c>
     </row>
-    <row r="17" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -9171,8 +9219,11 @@
       <c r="FJ17" s="4">
         <v>2.2294725394235964</v>
       </c>
+      <c r="FK17" s="4">
+        <v>2.1703743895822027</v>
+      </c>
     </row>
-    <row r="18" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -9671,8 +9722,11 @@
       <c r="FJ18" s="8">
         <v>2.5534132360604511</v>
       </c>
+      <c r="FK18" s="8">
+        <v>2.496099843993751</v>
+      </c>
     </row>
-    <row r="19" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -10169,10 +10223,13 @@
         <v>3.1649083842309924</v>
       </c>
       <c r="FJ19" s="8">
-        <v>3.2384142936906821</v>
+        <v>3.1825795644891222</v>
+      </c>
+      <c r="FK19" s="8">
+        <v>3.1666666666666607</v>
       </c>
     </row>
-    <row r="20" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
@@ -10671,8 +10728,11 @@
       <c r="FJ20" s="9">
         <v>2.5524673851389674</v>
       </c>
+      <c r="FK20" s="9">
+        <v>2.6704545454545392</v>
+      </c>
     </row>
-    <row r="21" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -11171,8 +11231,11 @@
       <c r="FJ21" s="4">
         <v>2.5569760978321256</v>
       </c>
+      <c r="FK21" s="4">
+        <v>2.6082130965593882</v>
+      </c>
     </row>
-    <row r="22" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -11669,10 +11732,13 @@
         <v>4.3410852713178318</v>
       </c>
       <c r="FJ22" s="4">
-        <v>4.4329896907216462</v>
+        <v>4.3814432989690717</v>
+      </c>
+      <c r="FK22" s="4">
+        <v>4.573484069886951</v>
       </c>
     </row>
-    <row r="23" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -12171,8 +12237,11 @@
       <c r="FJ23" s="4">
         <v>3.8992201559688064</v>
       </c>
+      <c r="FK23" s="4">
+        <v>2.1188934667451407</v>
+      </c>
     </row>
-    <row r="24" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -12671,8 +12740,11 @@
       <c r="FJ24" s="4">
         <v>2.5028441410693838</v>
       </c>
+      <c r="FK24" s="4">
+        <v>2.3823028927963632</v>
+      </c>
     </row>
-    <row r="25" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -13171,8 +13243,11 @@
       <c r="FJ25" s="4">
         <v>4.3665768194070056</v>
       </c>
+      <c r="FK25" s="4">
+        <v>4.0042712226374793</v>
+      </c>
     </row>
-    <row r="26" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -13669,10 +13744,13 @@
         <v>13.54062186559679</v>
       </c>
       <c r="FJ26" s="4">
-        <v>14.757378689344671</v>
+        <v>14.807403701850921</v>
+      </c>
+      <c r="FK26" s="4">
+        <v>15.119760479041908</v>
       </c>
     </row>
-    <row r="27" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -14171,8 +14249,11 @@
       <c r="FJ27" s="8">
         <v>5.4884742041712409</v>
       </c>
+      <c r="FK27" s="8">
+        <v>5.0081654872074131</v>
+      </c>
     </row>
-    <row r="28" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
@@ -14671,8 +14752,11 @@
       <c r="FJ28" s="9">
         <v>2.1030494216614093</v>
       </c>
+      <c r="FK28" s="9">
+        <v>1.5544041450777202</v>
+      </c>
     </row>
-    <row r="29" spans="1:166" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>48</v>
       </c>
@@ -15169,7 +15253,10 @@
         <v>4.1676335079544433</v>
       </c>
       <c r="FJ29" s="15">
-        <v>4.4468442601695903</v>
+        <v>4.3942252662043773</v>
+      </c>
+      <c r="FK29" s="15">
+        <v>3.9418786794032821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated arrivals and monthly cpi
</commit_message>
<xml_diff>
--- a/inflation_2012-24.xlsx
+++ b/inflation_2012-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RBI Official\DCA\Dashboard\Inflation-monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC922CD-DD10-4678-B269-842C7DA1D801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B9AB9F-5202-4D66-98D2-6C9A722246C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{3EA9A55A-B48B-4035-99BE-2980B3C8C172}"/>
   </bookViews>
@@ -658,13 +658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DBFB1-5D6A-4B75-89EE-EC9E4D2C9668}">
-  <dimension ref="A1:FK29"/>
+  <dimension ref="A1:FL29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="EQ2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="ET2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="FN7" sqref="FN7"/>
+      <selection pane="bottomRight" activeCell="FL2" sqref="FL2:FL29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,7 +672,7 @@
     <col min="1" max="1" width="6.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:167" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:168" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1174,8 +1174,11 @@
       <c r="FK1" s="16">
         <v>45839</v>
       </c>
+      <c r="FL1" s="16">
+        <v>45870</v>
+      </c>
     </row>
-    <row r="2" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1677,8 +1680,11 @@
       <c r="FK2" s="4">
         <v>3.0318870883429079</v>
       </c>
+      <c r="FL2" s="4">
+        <v>2.7027027027026964</v>
+      </c>
     </row>
-    <row r="3" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2180,8 +2186,11 @@
       <c r="FK3" s="4">
         <v>-0.60684872128304179</v>
       </c>
+      <c r="FL3" s="4">
+        <v>1.4778325123152631</v>
+      </c>
     </row>
-    <row r="4" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2681,10 +2690,13 @@
         <v>2.5748817656331986</v>
       </c>
       <c r="FK4" s="4">
-        <v>2.2645393721049802</v>
+        <v>2.2130725681935064</v>
+      </c>
+      <c r="FL4" s="4">
+        <v>3.1216931216931245</v>
       </c>
     </row>
-    <row r="5" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3184,10 +3196,13 @@
         <v>2.8047464940668765</v>
       </c>
       <c r="FK5" s="4">
-        <v>2.7419354838709649</v>
+        <v>2.6881720430107525</v>
+      </c>
+      <c r="FL5" s="4">
+        <v>2.6273458445040245</v>
       </c>
     </row>
-    <row r="6" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -3689,8 +3704,11 @@
       <c r="FK6" s="8">
         <v>19.242706393544385</v>
       </c>
+      <c r="FL6" s="8">
+        <v>21.238390092879264</v>
+      </c>
     </row>
-    <row r="7" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -4190,10 +4208,13 @@
         <v>12.642430819316322</v>
       </c>
       <c r="FK7" s="4">
-        <v>14.423592493297591</v>
+        <v>14.47721179624665</v>
+      </c>
+      <c r="FL7" s="4">
+        <v>11.650992685475435</v>
       </c>
     </row>
-    <row r="8" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -4693,10 +4714,13 @@
         <v>-18.915456874466262</v>
       </c>
       <c r="FK8" s="4">
-        <v>-20.688365132809579</v>
+        <v>-20.650953984287323</v>
+      </c>
+      <c r="FL8" s="4">
+        <v>-15.918680475642502</v>
       </c>
     </row>
-    <row r="9" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -5198,8 +5222,11 @@
       <c r="FK9" s="8">
         <v>-13.757604117922313</v>
       </c>
+      <c r="FL9" s="8">
+        <v>-14.53190498369818</v>
+      </c>
     </row>
-    <row r="10" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -5701,8 +5728,11 @@
       <c r="FK10" s="4">
         <v>3.2824427480916114</v>
       </c>
+      <c r="FL10" s="4">
+        <v>3.7290715372907193</v>
+      </c>
     </row>
-    <row r="11" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -6202,10 +6232,13 @@
         <v>-3.0303030303030205</v>
       </c>
       <c r="FK11" s="4">
-        <v>-3.0715225976305396</v>
+        <v>-3.1154014918824022</v>
+      </c>
+      <c r="FL11" s="4">
+        <v>-3.2441911442349869</v>
       </c>
     </row>
-    <row r="12" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -6707,8 +6740,11 @@
       <c r="FK12" s="4">
         <v>4.5964125560538047</v>
       </c>
+      <c r="FL12" s="4">
+        <v>4.2968750000000098</v>
+      </c>
     </row>
-    <row r="13" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -7208,10 +7244,13 @@
         <v>4.3176178660049569</v>
       </c>
       <c r="FK13" s="4">
-        <v>4.3542800593765518</v>
+        <v>4.4037605145967369</v>
+      </c>
+      <c r="FL13" s="4">
+        <v>4.1871921182266005</v>
       </c>
     </row>
-    <row r="14" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -7713,8 +7752,11 @@
       <c r="FK14" s="9">
         <v>-0.83620265617315148</v>
       </c>
+      <c r="FL14" s="9">
+        <v>4.9333991119892812E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
@@ -8216,8 +8258,11 @@
       <c r="FK15" s="8">
         <v>2.4495677233429505</v>
       </c>
+      <c r="FL15" s="8">
+        <v>2.4940047961630638</v>
+      </c>
     </row>
-    <row r="16" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -8719,8 +8764,11 @@
       <c r="FK16" s="4">
         <v>2.5826446280991737</v>
       </c>
+      <c r="FL16" s="4">
+        <v>2.4214322514168045</v>
+      </c>
     </row>
-    <row r="17" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -9222,8 +9270,11 @@
       <c r="FK17" s="4">
         <v>2.1703743895822027</v>
       </c>
+      <c r="FL17" s="4">
+        <v>2.0021645021644958</v>
+      </c>
     </row>
-    <row r="18" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -9725,8 +9776,11 @@
       <c r="FK18" s="8">
         <v>2.496099843993751</v>
       </c>
+      <c r="FL18" s="8">
+        <v>2.3340248962655603</v>
+      </c>
     </row>
-    <row r="19" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -10228,8 +10282,11 @@
       <c r="FK19" s="8">
         <v>3.1666666666666607</v>
       </c>
+      <c r="FL19" s="8">
+        <v>3.0922142462727744</v>
+      </c>
     </row>
-    <row r="20" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>0</v>
       </c>
@@ -10731,8 +10788,11 @@
       <c r="FK20" s="9">
         <v>2.6704545454545392</v>
       </c>
+      <c r="FL20" s="9">
+        <v>2.4335031126202669</v>
+      </c>
     </row>
-    <row r="21" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -11234,8 +11294,11 @@
       <c r="FK21" s="4">
         <v>2.6082130965593882</v>
       </c>
+      <c r="FL21" s="4">
+        <v>2.5428413488114949</v>
+      </c>
     </row>
-    <row r="22" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -11737,8 +11800,11 @@
       <c r="FK22" s="4">
         <v>4.573484069886951</v>
       </c>
+      <c r="FL22" s="4">
+        <v>4.4012282497441113</v>
+      </c>
     </row>
-    <row r="23" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -12240,8 +12306,11 @@
       <c r="FK23" s="4">
         <v>2.1188934667451407</v>
       </c>
+      <c r="FL23" s="4">
+        <v>1.936619718309849</v>
+      </c>
     </row>
-    <row r="24" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -12743,8 +12812,11 @@
       <c r="FK24" s="4">
         <v>2.3823028927963632</v>
       </c>
+      <c r="FL24" s="4">
+        <v>2.2033898305084776</v>
+      </c>
     </row>
-    <row r="25" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -13244,10 +13316,13 @@
         <v>4.3665768194070056</v>
       </c>
       <c r="FK25" s="4">
-        <v>4.0042712226374793</v>
+        <v>4.1110517885744731</v>
+      </c>
+      <c r="FL25" s="4">
+        <v>3.6036036036036099</v>
       </c>
     </row>
-    <row r="26" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -13749,8 +13824,11 @@
       <c r="FK26" s="4">
         <v>15.119760479041908</v>
       </c>
+      <c r="FL26" s="4">
+        <v>16.60830415207603</v>
+      </c>
     </row>
-    <row r="27" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -14252,8 +14330,11 @@
       <c r="FK27" s="8">
         <v>5.0081654872074131</v>
       </c>
+      <c r="FL27" s="8">
+        <v>5.0461204557786123</v>
+      </c>
     </row>
-    <row r="28" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>0</v>
       </c>
@@ -14753,10 +14834,13 @@
         <v>2.1030494216614093</v>
       </c>
       <c r="FK28" s="9">
-        <v>1.5544041450777202</v>
+        <v>1.6062176165803081</v>
+      </c>
+      <c r="FL28" s="9">
+        <v>2.0725388601036272</v>
       </c>
     </row>
-    <row r="29" spans="1:167" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:168" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>48</v>
       </c>
@@ -15256,7 +15340,10 @@
         <v>4.3942252662043773</v>
       </c>
       <c r="FK29" s="15">
-        <v>3.9418786794032821</v>
+        <v>4.0558670858704291</v>
+      </c>
+      <c r="FL29" s="15">
+        <v>4.1612178885913922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>